<commit_message>
Update files that contains blank column(index)
</commit_message>
<xml_diff>
--- a/Output/v3/scores_arima.xlsx
+++ b/Output/v3/scores_arima.xlsx
@@ -410,138 +410,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="B2">
         <v>0.08688570912085422</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="B3">
         <v>0.06346757147337655</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>0.07430544705601291</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="B5">
         <v>0.04070145528386912</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="B6">
         <v>0.02855885702341123</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="B7">
         <v>0.01749967251241708</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="B8">
         <v>0.07746537533108125</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="B9">
         <v>0.1705093227061947</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="B10">
         <v>0.06964792188795489</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
+      <c r="B11">
         <v>0.08924714421638058</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="C12">
+      <c r="B12">
         <v>0.1067133073111423</v>
       </c>
     </row>

</xml_diff>